<commit_message>
Implementação da Página de Listagem de Pedidos
</commit_message>
<xml_diff>
--- a/data/pedidos.xlsx
+++ b/data/pedidos.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -34,19 +34,19 @@
     <t>Jonas</t>
   </si>
   <si>
+    <t>Camisa</t>
+  </si>
+  <si>
+    <t>Novo</t>
+  </si>
+  <si>
+    <t>Calça</t>
+  </si>
+  <si>
+    <t>Sapato</t>
+  </si>
+  <si>
     <t>Maria</t>
-  </si>
-  <si>
-    <t>Camisa</t>
-  </si>
-  <si>
-    <t>Calça</t>
-  </si>
-  <si>
-    <t>Sapato</t>
-  </si>
-  <si>
-    <t>Novo</t>
   </si>
   <si>
     <t>Processando</t>
@@ -55,8 +55,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,10 +68,15 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,7 +87,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -91,34 +97,61 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+  <cellXfs count="7">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -127,10 +160,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -168,69 +201,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -254,54 +289,53 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
+                <a:tint val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
+                <a:tint val="15000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
+                <a:tint val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
+              <a:shade val="9500"/>
               <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -311,7 +345,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -320,7 +354,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -329,7 +363,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -337,10 +371,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -369,7 +403,7 @@
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
+                <a:tint val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
@@ -382,13 +416,12 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
@@ -406,112 +439,122 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4">
+        <v>50</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="4">
+        <v>80</v>
+      </c>
+      <c r="D3" s="4">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="4">
         <v>50</v>
       </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
-        <v>80</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C4">
+      <c r="C6" s="4">
         <v>100</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>50</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
-        <v>100</v>
-      </c>
-      <c r="D6">
+      <c r="D6" s="4">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>